<commit_message>
Se ha corregido la portada del reporte y las imágenes de los resultados de validación cruzada
</commit_message>
<xml_diff>
--- a/Desarrollo/Clasificador/Resultados/Prueba.08.10.2019/Reporte/Graficas/Matriz_De_Resultados.xlsx
+++ b/Desarrollo/Clasificador/Resultados/Prueba.08.10.2019/Reporte/Graficas/Matriz_De_Resultados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andrew/Documents/ESCOM/TT2/TT2/Desarrollo/Clasificador/Resultados/Prueba.08.10.2019/Reporte/Graficas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0919CC48-E950-2544-9B36-E378D9EB364A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DFE906-E937-7B49-97D2-EB41A2AA52A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{95AA4C3A-DABF-B14D-92ED-AB883A3C489A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{95AA4C3A-DABF-B14D-92ED-AB883A3C489A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -73,25 +73,13 @@
   </si>
   <si>
     <t>Random forest</t>
-  </si>
-  <si>
-    <t>Accuracy Promedio(%)</t>
-  </si>
-  <si>
-    <t>Fmeaseure Promedio(%)</t>
-  </si>
-  <si>
-    <t>Recall Promedio(%)</t>
-  </si>
-  <si>
-    <t>Precision Promedio(%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,14 +96,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
+      <sz val="16"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -123,7 +104,28 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Avenir Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Avenir Book"/>
       <family val="2"/>
@@ -177,25 +179,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -520,12 +523,12 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
@@ -534,255 +537,273 @@
     <col min="8" max="8" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="2:8" ht="40" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="2:8" ht="44" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="26" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>2844</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="5">
         <v>3447</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="6">
         <v>0.82499999999999996</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="6">
         <v>0.82599999999999996</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="6">
         <v>0.83699999999999997</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="6">
         <v>0.82599999999999996</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="63" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:8" ht="72" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>2947</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="5">
         <v>3447</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>0.85399999999999998</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
         <v>0.85499999999999998</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="6">
         <v>0.85599999999999998</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="6">
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="2:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>2898</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="5">
         <v>3447</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>0.84</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="6">
         <v>0.84099999999999997</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="6">
         <v>0.84099999999999997</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="6">
         <v>0.84199999999999997</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="42" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="5">
         <v>3001</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="5">
         <v>3447</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>0.87</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="6">
         <v>0.871</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="6">
         <v>0.872</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="6">
         <v>0.871</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+    <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="2:8" ht="40" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="2:8" ht="44" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="2:8" ht="26" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="5">
         <v>2877</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="5">
         <v>3447</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="6">
         <v>0.83399999999999996</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="6">
         <v>0.83499999999999996</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="6">
         <v>0.84399999999999997</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="6">
         <v>0.83599999999999997</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="63" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:8" ht="72" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="5">
         <v>2684</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="5">
         <v>3447</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="6">
         <v>0.77800000000000002</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="6">
         <v>0.78100000000000003</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="6">
         <v>0.78700000000000003</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="6">
         <v>0.77900000000000003</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="42" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="2:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="5">
         <v>2878</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="5">
         <v>3447</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="6">
         <v>0.83399999999999996</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="6">
         <v>0.83399999999999996</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="6">
         <v>0.83599999999999997</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="6">
         <v>0.83599999999999997</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="42" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="2:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="5">
         <v>2983</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="5">
         <v>3447</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="6">
         <v>0.86</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="6">
         <v>0.86</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="6">
         <v>0.86</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="6">
         <v>0.86</v>
       </c>
     </row>

</xml_diff>